<commit_message>
cleared the dt_reason tab
</commit_message>
<xml_diff>
--- a/files/PH_Configuration_Dev.xlsx
+++ b/files/PH_Configuration_Dev.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rf128sp\Desktop\Smart Factory\Parker Hannifin\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rf128sp\ADV-DXH\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6950" firstSheet="3" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6950"/>
   </bookViews>
   <sheets>
     <sheet name="dt_reason" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="49">
   <si>
     <t>code</t>
   </si>
@@ -60,45 +60,6 @@
   </si>
   <si>
     <t>status</t>
-  </si>
-  <si>
-    <t>O-Ring Detection Setup</t>
-  </si>
-  <si>
-    <t>Short Packing Supplies</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wrong Part/Component/O-ring etc </t>
-  </si>
-  <si>
-    <t>Short Part/Component/O-ring etc</t>
-  </si>
-  <si>
-    <t>Meeting/Training</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Label /Assembly Instruction /Paperwork Error </t>
-  </si>
-  <si>
-    <t>Ran out of work</t>
-  </si>
-  <si>
-    <t>Parts Rejected/Quality Inspection/Rework(Plating/Machining)</t>
-  </si>
-  <si>
-    <t>5S</t>
-  </si>
-  <si>
-    <t>Setup - Hard Assembly</t>
-  </si>
-  <si>
-    <t>1 in a box</t>
-  </si>
-  <si>
-    <t>Multiple small jobs</t>
-  </si>
-  <si>
-    <t>Other - Please Specify</t>
   </si>
   <si>
     <t>site_code</t>
@@ -605,10 +566,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -647,110 +608,6 @@
       </c>
       <c r="J1" s="3" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="G2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="G3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="G4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="G5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="G6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="G7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="G8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="G9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="G10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="G11" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="G12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="G13" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="G14" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -780,40 +637,40 @@
         <v>5</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="K1" s="4" t="s">
         <v>9</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -845,46 +702,46 @@
   <sheetData>
     <row r="1" spans="1:14" s="5" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>5</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="L1" s="4" t="s">
         <v>9</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -896,7 +753,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
@@ -912,46 +769,46 @@
   <sheetData>
     <row r="1" spans="1:14" s="5" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>5</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="L1" s="4" t="s">
         <v>9</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -977,13 +834,13 @@
   <sheetData>
     <row r="1" spans="1:7" s="5" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>4</v>
@@ -992,10 +849,10 @@
         <v>9</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -1019,22 +876,22 @@
   <sheetData>
     <row r="1" spans="1:6" s="5" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -1060,28 +917,28 @@
   <sheetData>
     <row r="1" spans="1:12" s="5" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>5</v>
@@ -1090,10 +947,10 @@
         <v>9</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added missing attributes to the tables
</commit_message>
<xml_diff>
--- a/files/PH_Configuration_Dev.xlsx
+++ b/files/PH_Configuration_Dev.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6950"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6950" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="dt_reason" sheetId="1" r:id="rId1"/>
@@ -30,19 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="49">
-  <si>
-    <t>code</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>color</t>
-  </si>
-  <si>
-    <t>category</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="60">
   <si>
     <t>value</t>
   </si>
@@ -89,12 +77,6 @@
     <t>grouping3</t>
   </si>
   <si>
-    <t>timestamp</t>
-  </si>
-  <si>
-    <t>message_source</t>
-  </si>
-  <si>
     <t>valid_from</t>
   </si>
   <si>
@@ -161,15 +143,6 @@
     <t>parameter_description</t>
   </si>
   <si>
-    <t>uom_code</t>
-  </si>
-  <si>
-    <t>uom_name</t>
-  </si>
-  <si>
-    <t>uom_description</t>
-  </si>
-  <si>
     <t>unavailable_code</t>
   </si>
   <si>
@@ -177,6 +150,66 @@
   </si>
   <si>
     <t>unavailable_description</t>
+  </si>
+  <si>
+    <t>asset_id</t>
+  </si>
+  <si>
+    <t>automation_level</t>
+  </si>
+  <si>
+    <t>entered_by</t>
+  </si>
+  <si>
+    <t>entered_on</t>
+  </si>
+  <si>
+    <t>last_modified_by</t>
+  </si>
+  <si>
+    <t>last_modified_on</t>
+  </si>
+  <si>
+    <t>parameter_id</t>
+  </si>
+  <si>
+    <t>dtreason_id</t>
+  </si>
+  <si>
+    <t>dtreason_code</t>
+  </si>
+  <si>
+    <t>dtreason_name</t>
+  </si>
+  <si>
+    <t>dtreason_description</t>
+  </si>
+  <si>
+    <t>dtreason_category</t>
+  </si>
+  <si>
+    <t>tag_value</t>
+  </si>
+  <si>
+    <t>shift_id</t>
+  </si>
+  <si>
+    <t>tag_id</t>
+  </si>
+  <si>
+    <t>UOM_code</t>
+  </si>
+  <si>
+    <t>unavailable_id</t>
+  </si>
+  <si>
+    <t>UOM_id</t>
+  </si>
+  <si>
+    <t>UOM_name</t>
+  </si>
+  <si>
+    <t>UOM_description</t>
   </si>
 </sst>
 </file>
@@ -566,48 +599,68 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:O1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="6" max="6" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="52.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.90625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.6328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="K1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>9</v>
+      <c r="L1" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -618,59 +671,73 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:Q1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1:Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.36328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.6328125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="5" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" s="5" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="M1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>20</v>
+      <c r="N1" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -680,68 +747,77 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N1"/>
+  <dimension ref="A1:Q1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.08984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.36328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.7265625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.26953125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="4.36328125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.26953125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.36328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.7265625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.36328125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="5" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" s="5" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>27</v>
+        <v>53</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="I1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="M1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>19</v>
-      </c>
       <c r="N1" s="4" t="s">
-        <v>20</v>
+        <v>42</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -751,64 +827,75 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N1"/>
+  <dimension ref="A1:Q1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1:Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.26953125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="4.36328125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.26953125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.36328125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.90625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="5" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" s="5" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="J1" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="K1" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="I1" s="4" t="s">
+      <c r="N1" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="O1" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="J1" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>20</v>
+      <c r="P1" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -818,41 +905,53 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.90625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="5" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="5" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>20</v>
+      <c r="H1" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -862,36 +961,48 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="F1" sqref="F1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.90625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="5" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="5" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>45</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -901,56 +1012,70 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:O1"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1:O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="15.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.08984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.81640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.6328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.08984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.90625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="5" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="5" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="I1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>19</v>
-      </c>
       <c r="L1" s="4" t="s">
-        <v>20</v>
+        <v>42</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed order assembly and sorting logic in API
</commit_message>
<xml_diff>
--- a/files/PH_Configuration_Dev.xlsx
+++ b/files/PH_Configuration_Dev.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rf128sp\ADV-DXH\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32531825-363F-438D-B505-E82E8499D3C7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D26A8617-D4BE-4AF0-9EBF-798526ED64E6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6945" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="dt_reason" sheetId="1" r:id="rId1"/>
+    <sheet name="dtreason" sheetId="1" r:id="rId1"/>
     <sheet name="asset" sheetId="2" r:id="rId2"/>
     <sheet name="shift" sheetId="3" r:id="rId3"/>
     <sheet name="tag" sheetId="4" r:id="rId4"/>

</xml_diff>